<commit_message>
Updates to tabular data
</commit_message>
<xml_diff>
--- a/tabular/eve/efv-refseq-side-data.xlsx
+++ b/tabular/eve/efv-refseq-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298E4B9D-DDC8-6746-8FBA-072C82C5A2EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AD696B-72CD-7D40-9781-E6DF09B74D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="28060" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17520" yWindow="460" windowWidth="33580" windowHeight="25220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="156">
   <si>
     <t>In project?</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>Bee</t>
+  </si>
+  <si>
+    <t>EFV-PL2.8-EusHer</t>
   </si>
 </sst>
 </file>
@@ -511,9 +514,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +523,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -551,7 +553,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,12 +568,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -579,24 +575,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.24994659260841701"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,33 +605,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -987,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,13 +968,13 @@
     <col min="2" max="5" width="24.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" style="6" customWidth="1"/>
     <col min="9" max="9" width="20.1640625" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" customWidth="1"/>
     <col min="11" max="11" width="30.5" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="16" style="11" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="16" style="6" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1031,10 +1000,10 @@
       <c r="G1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1046,10 +1015,10 @@
       <c r="L1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -1060,1690 +1029,1766 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="7">
         <v>10</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="7">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>16</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P3" s="3" t="s">
+      <c r="O3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="7">
         <v>3</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="I4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="7">
         <v>1</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="O4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <v>4</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" t="s">
+      <c r="K5" s="8"/>
+      <c r="L5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="7">
         <v>1</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P5" s="3" t="s">
+      <c r="O5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>5</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="7">
         <v>4</v>
       </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P6" s="3" t="s">
+      <c r="N6" s="7"/>
+      <c r="O6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>6</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="I7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="7">
         <v>1</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="3" t="s">
+      <c r="O7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>1</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="I8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="7">
         <v>7</v>
       </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P8" s="3" t="s">
+      <c r="N8" s="7"/>
+      <c r="O8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <v>2</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="I9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="7">
         <v>2</v>
       </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P9" s="3" t="s">
+      <c r="N9" s="7"/>
+      <c r="O9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <v>3</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="7">
         <v>3</v>
       </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P10" s="3" t="s">
+      <c r="N10" s="7"/>
+      <c r="O10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>1</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="I11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="7">
         <v>1</v>
       </c>
-      <c r="N11" s="13" t="s">
+      <c r="N11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P11" s="3" t="s">
+      <c r="O11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>2</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="I12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="7">
         <v>2</v>
       </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P12" s="3" t="s">
+      <c r="N12" s="7"/>
+      <c r="O12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <v>3</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="I13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="7">
         <v>2</v>
       </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P13" s="3" t="s">
+      <c r="N13" s="7"/>
+      <c r="O13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="7">
         <v>4</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J14" s="3" t="s">
+      <c r="I14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="7">
         <v>1</v>
       </c>
-      <c r="N14" s="13" t="s">
+      <c r="N14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P14" s="3" t="s">
+      <c r="O14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="7">
         <v>1</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="I15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="7">
         <v>2</v>
       </c>
-      <c r="N15" s="13"/>
-      <c r="O15" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P15" s="3" t="s">
+      <c r="N15" s="7"/>
+      <c r="O15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="7">
         <v>1</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="I16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="7">
         <v>6</v>
       </c>
-      <c r="N16" s="13"/>
-      <c r="O16" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P16" s="3" t="s">
+      <c r="N16" s="7"/>
+      <c r="O16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="7">
         <v>2</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="I17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="7">
         <v>4</v>
       </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P17" s="3" t="s">
+      <c r="N17" s="7"/>
+      <c r="O17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="7">
         <v>3</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="I18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="7">
         <v>1</v>
       </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P18" s="3" t="s">
+      <c r="N18" s="7"/>
+      <c r="O18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="7">
         <v>1</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J19" s="3" t="s">
+      <c r="I19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P19" s="3" t="s">
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="E20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="7">
         <v>2</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="I20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P20" s="3" t="s">
+      <c r="M20" s="7">
+        <v>1</v>
+      </c>
+      <c r="N20" s="7"/>
+      <c r="O20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="E21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="7">
         <v>3</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J21" s="3" t="s">
+      <c r="I21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P21" s="3" t="s">
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P21" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="E22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="7">
         <v>3</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J22" s="3" t="s">
+      <c r="I22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P22" s="3" t="s">
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P22" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="E23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="7">
         <v>3</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" s="3" t="s">
+      <c r="I23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P23" s="3" t="s">
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="E24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="7">
         <v>3</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="I24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P24" s="3" t="s">
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P24" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="5" t="s">
+      <c r="E25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="7">
         <v>3</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="I25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O25" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P25" s="3" t="s">
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P25" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="E26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="7">
         <v>3</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J26" s="3" t="s">
+      <c r="I26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P26" s="3" t="s">
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27" s="7">
         <v>3</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="I27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P27" s="3" t="s">
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P27" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="E28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="7">
         <v>3</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J28" s="3" t="s">
+      <c r="I28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O28" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P28" s="3" t="s">
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P28" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="E29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="7">
         <v>3</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="I29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O29" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P29" s="3" t="s">
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P29" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" s="5" t="s">
+      <c r="E30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="7">
         <v>4</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J30" s="3" t="s">
+      <c r="I30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="7">
         <v>2</v>
       </c>
-      <c r="N30" s="13"/>
-      <c r="O30" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P30" s="3" t="s">
+      <c r="N30" s="7"/>
+      <c r="O30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P30" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="E31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H31" s="7">
         <v>5</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="I31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P31" s="3" t="s">
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P31" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F32" s="5" t="s">
+      <c r="E32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H32" s="10">
+      <c r="H32" s="7">
         <v>6</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J32" s="3" t="s">
+      <c r="I32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="7">
         <v>16</v>
       </c>
-      <c r="N32" s="13"/>
-      <c r="O32" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P32" s="3" t="s">
+      <c r="N32" s="7"/>
+      <c r="O32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P32" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H33" s="10">
+      <c r="H33" s="7">
         <v>7</v>
       </c>
-      <c r="I33" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J33" s="3" t="s">
+      <c r="I33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="K33" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="L33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="7">
         <v>2</v>
       </c>
-      <c r="N33" s="13"/>
-      <c r="O33" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P33" s="3" t="s">
+      <c r="N33" s="7"/>
+      <c r="O33" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P33" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" s="7">
+        <v>9</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M34" s="7">
+        <v>1</v>
+      </c>
+      <c r="N34" s="7"/>
+      <c r="O34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E35" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F35" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H35" s="7">
         <v>1</v>
       </c>
-      <c r="I34" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="I35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K35" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="L35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M35" s="7">
         <v>1</v>
       </c>
-      <c r="O34" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P34" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="N35" s="7"/>
+      <c r="O35" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F35" s="5" t="s">
+      <c r="E36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H35" s="10">
+      <c r="H36" s="7">
         <v>1</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K36" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="L36" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M36" s="7">
         <v>2</v>
       </c>
-      <c r="O35" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P35" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="N36" s="7"/>
+      <c r="O36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="5" t="s">
+      <c r="E37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H37" s="7">
         <v>2</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="I37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K37" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="L36" s="3" t="s">
+      <c r="L37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M37" s="7">
         <v>1</v>
       </c>
-      <c r="O36" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P36" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="N37" s="7"/>
+      <c r="O37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37" s="5" t="s">
+      <c r="E38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G38" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H38" s="7">
         <v>1</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="I38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K38" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="L37" s="3" t="s">
+      <c r="L38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M38" s="7">
         <v>1</v>
       </c>
-      <c r="O37" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P37" s="3" t="s">
+      <c r="N38" s="7"/>
+      <c r="O38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P38" s="2" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2794,123 +2839,123 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>1</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>3</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding pestivirus EVE to project
</commit_message>
<xml_diff>
--- a/tabular/eve/efv-refseq-side-data.xlsx
+++ b/tabular/eve/efv-refseq-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D963F06A-43C0-4047-BE41-592960FCBE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4991780-9387-5C45-B72C-214D83B87C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="4900" windowWidth="27940" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="172">
   <si>
     <t>In project?</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Operophtera brumata</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Flavivirus</t>
   </si>
   <si>
@@ -537,26 +534,31 @@
   </si>
   <si>
     <t>EFV-PL2.8-AnoPla</t>
+  </si>
+  <si>
+    <t>EFV-Pesti.1-Crocidurinae</t>
+  </si>
+  <si>
+    <t>Pestivirus</t>
+  </si>
+  <si>
+    <t>Crocidurinae-Soricinae</t>
+  </si>
+  <si>
+    <t>Crocidurid &amp; Soricinid shrews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -644,29 +646,29 @@
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -675,7 +677,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1012,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E12" sqref="E9:E12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="L28" sqref="A1:Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,99 +1031,95 @@
     <col min="13" max="13" width="30.5" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="16" style="5" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>0</v>
+      <c r="P1" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J2" s="6">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>2</v>
@@ -1131,54 +1128,51 @@
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O2" s="6">
         <v>10</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J3" s="6">
         <v>2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>5</v>
@@ -1187,162 +1181,153 @@
         <v>4</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="6">
         <v>16</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J4" s="6">
         <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4" s="6">
         <v>1</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>61</v>
+      <c r="P4" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J5" s="6">
         <v>4</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O5" s="6">
         <v>1</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>61</v>
+      <c r="P5" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J6" s="6">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>7</v>
@@ -1351,162 +1336,157 @@
         <v>6</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O6" s="6">
         <v>4</v>
       </c>
-      <c r="P6" s="6"/>
+      <c r="P6" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J7" s="6">
         <v>6</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O7" s="6">
         <v>1</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>61</v>
+      <c r="P7" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J8" s="6">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O8" s="6">
         <v>7</v>
       </c>
-      <c r="P8" s="6"/>
+      <c r="P8" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q8" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J9" s="6">
         <v>2</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>9</v>
@@ -1515,52 +1495,51 @@
         <v>8</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O9" s="6">
         <v>2</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="P9" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q9" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J10" s="6">
         <v>3</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>12</v>
@@ -1569,268 +1548,263 @@
         <v>11</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O10" s="6">
         <v>3</v>
       </c>
-      <c r="P10" s="6"/>
+      <c r="P10" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q10" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J11" s="6">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M11" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="N11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O11" s="6">
         <v>1</v>
       </c>
-      <c r="P11" s="6"/>
+      <c r="P11" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J12" s="6">
         <v>1</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O12" s="6">
         <v>2</v>
       </c>
-      <c r="P12" s="6"/>
+      <c r="P12" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q12" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="6">
         <v>2</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O13" s="6">
         <v>1</v>
       </c>
-      <c r="P13" s="6"/>
+      <c r="P13" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q13" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J14" s="6">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O14" s="6">
         <v>1</v>
       </c>
-      <c r="P14" s="6"/>
+      <c r="P14" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q14" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J15" s="6">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>31</v>
@@ -1839,50 +1813,49 @@
         <v>30</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="P15" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J16" s="6">
         <v>2</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>34</v>
@@ -1891,210 +1864,206 @@
         <v>33</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O16" s="6">
         <v>1</v>
       </c>
-      <c r="P16" s="6"/>
+      <c r="P16" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J17" s="6">
         <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="M17" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="N17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="P17" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J18" s="6">
         <v>4</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>51</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O18" s="6">
         <v>2</v>
       </c>
-      <c r="P18" s="6"/>
+      <c r="P18" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q18" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J19" s="6">
         <v>5</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="M19" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="N19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="P19" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q19" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J20" s="6">
         <v>6</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>53</v>
@@ -2103,52 +2072,51 @@
         <v>52</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O20" s="6">
         <v>16</v>
       </c>
-      <c r="P20" s="6"/>
+      <c r="P20" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q20" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J21" s="6">
         <v>7</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>55</v>
@@ -2157,52 +2125,51 @@
         <v>54</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O21" s="6">
         <v>2</v>
       </c>
-      <c r="P21" s="6"/>
+      <c r="P21" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J22" s="6">
         <v>9</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>34</v>
@@ -2211,108 +2178,104 @@
         <v>33</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O22" s="6">
         <v>1</v>
       </c>
-      <c r="P22" s="6"/>
+      <c r="P22" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J23" s="6">
         <v>1</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="M23" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="N23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O23" s="6">
         <v>1</v>
       </c>
-      <c r="P23" s="6" t="s">
-        <v>61</v>
+      <c r="P23" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J24" s="6">
         <v>2</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>16</v>
@@ -2321,52 +2284,51 @@
         <v>15</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O24" s="6">
         <v>2</v>
       </c>
-      <c r="P24" s="6"/>
+      <c r="P24" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J25" s="6">
         <v>3</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>19</v>
@@ -2375,52 +2337,51 @@
         <v>18</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O25" s="6">
         <v>2</v>
       </c>
-      <c r="P25" s="6"/>
+      <c r="P25" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q25" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J26" s="6">
         <v>4</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>21</v>
@@ -2429,39 +2390,36 @@
         <v>20</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O26" s="6">
         <v>1</v>
       </c>
-      <c r="P26" s="6" t="s">
-        <v>61</v>
+      <c r="P26" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>24</v>
@@ -2470,13 +2428,13 @@
         <v>24</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J27" s="6">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>23</v>
@@ -2485,37 +2443,36 @@
         <v>22</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O27" s="6">
         <v>2</v>
       </c>
-      <c r="P27" s="6"/>
+      <c r="P27" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q27" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>27</v>
@@ -2524,13 +2481,13 @@
         <v>27</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J28" s="6">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>29</v>
@@ -2539,37 +2496,36 @@
         <v>28</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O28" s="6">
         <v>6</v>
       </c>
-      <c r="P28" s="6"/>
+      <c r="P28" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q28" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>27</v>
@@ -2578,13 +2534,13 @@
         <v>27</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J29" s="6">
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>26</v>
@@ -2593,37 +2549,36 @@
         <v>25</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O29" s="6">
         <v>4</v>
       </c>
-      <c r="P29" s="6"/>
+      <c r="P29" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>27</v>
@@ -2632,13 +2587,13 @@
         <v>27</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J30" s="6">
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>21</v>
@@ -2647,37 +2602,36 @@
         <v>20</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O30" s="6">
         <v>1</v>
       </c>
-      <c r="P30" s="6"/>
+      <c r="P30" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q30" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>27</v>
@@ -2686,52 +2640,51 @@
         <v>27</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J31" s="6">
         <v>4</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O31" s="6">
         <v>1</v>
       </c>
-      <c r="P31" s="6"/>
+      <c r="P31" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q31" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>27</v>
@@ -2740,52 +2693,51 @@
         <v>27</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J32" s="6">
         <v>5</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O32" s="6">
         <v>1</v>
       </c>
-      <c r="P32" s="6"/>
+      <c r="P32" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q32" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>27</v>
@@ -2794,52 +2746,51 @@
         <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J33" s="6">
         <v>6</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O33" s="6">
         <v>1</v>
       </c>
-      <c r="P33" s="6"/>
+      <c r="P33" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q33" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>27</v>
@@ -2848,52 +2799,51 @@
         <v>27</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J34" s="6">
         <v>7</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L34" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M34" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="M34" s="8" t="s">
-        <v>150</v>
-      </c>
       <c r="N34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O34" s="6">
         <v>1</v>
       </c>
-      <c r="P34" s="6"/>
+      <c r="P34" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>27</v>
@@ -2902,52 +2852,51 @@
         <v>27</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J35" s="6">
         <v>8</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O35" s="6">
         <v>1</v>
       </c>
-      <c r="P35" s="6"/>
+      <c r="P35" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q35" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>27</v>
@@ -2956,95 +2905,144 @@
         <v>27</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J36" s="6">
         <v>9</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O36" s="6">
         <v>1</v>
       </c>
-      <c r="P36" s="6"/>
+      <c r="P36" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q36" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J37" s="5">
+        <v>118</v>
+      </c>
+      <c r="J37" s="6">
         <v>8</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="M37" s="10" t="s">
-        <v>70</v>
-      </c>
       <c r="N37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O37" s="6">
         <v>1</v>
       </c>
-      <c r="P37" s="6"/>
+      <c r="P37" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q37" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J38" s="6">
+        <v>1</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O38" s="6">
+        <v>26</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q36">
     <sortCondition ref="G2:G36"/>
     <sortCondition ref="H2:H36"/>
     <sortCondition ref="J2:J36"/>
   </sortState>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -3067,72 +3065,72 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>3</v>
@@ -3141,46 +3139,46 @@
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M2" s="6">
         <v>1</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>3</v>
@@ -3189,142 +3187,142 @@
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M3" s="6">
         <v>1</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H4" s="6">
         <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M4" s="6">
         <v>1</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M5" s="6">
         <v>1</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>3</v>
@@ -3333,28 +3331,28 @@
         <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M6" s="6">
         <v>1</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3377,81 +3375,81 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H2" s="6">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>36</v>
@@ -3460,44 +3458,44 @@
         <v>35</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H3" s="6">
         <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>38</v>
@@ -3506,44 +3504,44 @@
         <v>37</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="6">
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>40</v>
@@ -3552,44 +3550,44 @@
         <v>39</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" s="6">
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>42</v>
@@ -3598,44 +3596,44 @@
         <v>41</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" s="6">
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>44</v>
@@ -3644,44 +3642,44 @@
         <v>43</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" s="6">
         <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>46</v>
@@ -3690,44 +3688,44 @@
         <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H8" s="6">
         <v>3</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>48</v>
@@ -3736,44 +3734,44 @@
         <v>47</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H9" s="6">
         <v>3</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>50</v>
@@ -3782,15 +3780,15 @@
         <v>49</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>